<commit_message>
EPBDS: updated bean mapper.
</commit_message>
<xml_diff>
--- a/Util/trunk/openl-bean-mapper/src/test/resources/org/openl/mapper/RulesBeanMapperTest.xlsx
+++ b/Util/trunk/openl-bean-mapper/src/test/resources/org/openl/mapper/RulesBeanMapperTest.xlsx
@@ -91,9 +91,6 @@
     <t>d</t>
   </si>
   <si>
-    <t>Data Mapping mappings2</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>org.openl.mapper.model</t>
+  </si>
+  <si>
+    <t>Data Mapping mappings2</t>
   </si>
 </sst>
 </file>
@@ -507,10 +507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:H33"/>
+  <dimension ref="C4:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:D33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -534,7 +534,7 @@
     </row>
     <row r="5" spans="3:8" ht="149.25" customHeight="1">
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -670,7 +670,7 @@
     </row>
     <row r="22" spans="3:8">
       <c r="C22" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -720,10 +720,10 @@
     </row>
     <row r="25" spans="3:8">
       <c r="C25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>22</v>
@@ -752,38 +752,34 @@
     </row>
     <row r="30" spans="3:8">
       <c r="C30" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="3:8">
       <c r="C31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="32" spans="3:8">
       <c r="C32" s="4"/>
       <c r="D32" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4">
-      <c r="C33" s="4"/>
-      <c r="D33" s="2"/>
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="C22:H22"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS: updated mapper test.
</commit_message>
<xml_diff>
--- a/Util/trunk/openl-bean-mapper/src/test/resources/org/openl/mapper/RulesBeanMapperTest.xlsx
+++ b/Util/trunk/openl-bean-mapper/src/test/resources/org/openl/mapper/RulesBeanMapperTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
   <si>
     <t>classA</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Data Mapping mappings2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>x[1]</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,15 +178,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -486,7 +507,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
@@ -510,7 +531,7 @@
   <dimension ref="C4:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -527,38 +548,38 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:8">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="3:8" ht="149.25" customHeight="1">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="7" spans="3:8">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="3:8" ht="78.75" customHeight="1">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="12" spans="3:8">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="3:8">
       <c r="C13" s="2" t="s">
@@ -669,14 +690,14 @@
       <c r="H18" s="2"/>
     </row>
     <row r="22" spans="3:8">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="3:8">
       <c r="C23" s="2" t="s">
@@ -750,14 +771,28 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
+    <row r="27" spans="3:8">
+      <c r="C27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="30" spans="3:8">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="3:8">
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -765,21 +800,21 @@
       </c>
     </row>
     <row r="32" spans="3:8">
-      <c r="C32" s="4"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="C22:H22"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>